<commit_message>
28/01 second commit: after knitting
</commit_message>
<xml_diff>
--- a/_site/posts/2021-01-06-dataviz-makeover-1/data/mrsd_2019LabourForce_T7.xlsx
+++ b/_site/posts/2021-01-06-dataviz-makeover-1/data/mrsd_2019LabourForce_T7.xlsx
@@ -1,47 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421CBD32-5B8A-49E5-BF19-ED694CA757AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7100"/>
+    <workbookView xWindow="-28080" yWindow="1965" windowWidth="20520" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="T7_T" sheetId="1" r:id="rId1"/>
-    <sheet name="T7_M" sheetId="2" r:id="rId2"/>
-    <sheet name="T7_F" sheetId="3" r:id="rId3"/>
+    <sheet name="flat_pivot" sheetId="5" r:id="rId1"/>
+    <sheet name="flat" sheetId="4" r:id="rId2"/>
+    <sheet name="T7_T" sheetId="1" r:id="rId3"/>
+    <sheet name="T7_M" sheetId="2" r:id="rId4"/>
+    <sheet name="T7_F" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_Regression_Int" localSheetId="2" hidden="1">1</definedName>
     <definedName name="_Regression_Int" localSheetId="1" hidden="1">1</definedName>
     <definedName name="_Regression_Int" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="a" localSheetId="2">#REF!</definedName>
+    <definedName name="_Regression_Int" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="_Regression_Int" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="_Regression_Int" localSheetId="2" hidden="1">1</definedName>
     <definedName name="a" localSheetId="1">#REF!</definedName>
     <definedName name="a" localSheetId="0">#REF!</definedName>
+    <definedName name="a" localSheetId="4">#REF!</definedName>
+    <definedName name="a" localSheetId="3">#REF!</definedName>
+    <definedName name="a" localSheetId="2">#REF!</definedName>
     <definedName name="a">#REF!</definedName>
-    <definedName name="Economically_Inactive" localSheetId="2">#REF!</definedName>
     <definedName name="Economically_Inactive" localSheetId="1">#REF!</definedName>
     <definedName name="Economically_Inactive" localSheetId="0">#REF!</definedName>
+    <definedName name="Economically_Inactive" localSheetId="4">#REF!</definedName>
+    <definedName name="Economically_Inactive" localSheetId="3">#REF!</definedName>
+    <definedName name="Economically_Inactive" localSheetId="2">#REF!</definedName>
     <definedName name="Economically_Inactive">#REF!</definedName>
-    <definedName name="Employed" localSheetId="2">#REF!</definedName>
     <definedName name="Employed" localSheetId="1">#REF!</definedName>
     <definedName name="Employed" localSheetId="0">#REF!</definedName>
+    <definedName name="Employed" localSheetId="4">#REF!</definedName>
+    <definedName name="Employed" localSheetId="3">#REF!</definedName>
+    <definedName name="Employed" localSheetId="2">#REF!</definedName>
     <definedName name="Employed">#REF!</definedName>
-    <definedName name="Print_Area_MI" localSheetId="2">T7_F!$B$1:$Z$19</definedName>
-    <definedName name="Print_Area_MI" localSheetId="1">T7_M!$B$1:$Z$19</definedName>
-    <definedName name="Print_Area_MI" localSheetId="0">T7_T!$B$1:$Z$19</definedName>
+    <definedName name="Print_Area_MI" localSheetId="1">flat!$A$1:$L$14</definedName>
+    <definedName name="Print_Area_MI" localSheetId="0">flat_pivot!#REF!</definedName>
+    <definedName name="Print_Area_MI" localSheetId="4">T7_F!$B$1:$Z$19</definedName>
+    <definedName name="Print_Area_MI" localSheetId="3">T7_M!$B$1:$Z$19</definedName>
+    <definedName name="Print_Area_MI" localSheetId="2">T7_T!$B$1:$Z$19</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
-    <definedName name="Table" localSheetId="2">#REF!</definedName>
     <definedName name="Table" localSheetId="1">#REF!</definedName>
     <definedName name="Table" localSheetId="0">#REF!</definedName>
+    <definedName name="Table" localSheetId="4">#REF!</definedName>
+    <definedName name="Table" localSheetId="3">#REF!</definedName>
+    <definedName name="Table" localSheetId="2">#REF!</definedName>
     <definedName name="Table">#REF!</definedName>
-    <definedName name="Unemployed" localSheetId="2">#REF!</definedName>
     <definedName name="Unemployed" localSheetId="1">#REF!</definedName>
     <definedName name="Unemployed" localSheetId="0">#REF!</definedName>
+    <definedName name="Unemployed" localSheetId="4">#REF!</definedName>
+    <definedName name="Unemployed" localSheetId="3">#REF!</definedName>
+    <definedName name="Unemployed" localSheetId="2">#REF!</definedName>
     <definedName name="Unemployed">#REF!</definedName>
-    <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="2">#REF!</definedName>
     <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="1">#REF!</definedName>
     <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="0">#REF!</definedName>
+    <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="4">#REF!</definedName>
+    <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="3">#REF!</definedName>
+    <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by" localSheetId="2">#REF!</definedName>
     <definedName name="Unemployed_Residents_Aged_Fifteen_Years_and_Over_by">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -54,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>Source:  Comprehensive Labour Force Survey, Manpower Research &amp; Statistics Department, MOM</t>
   </si>
@@ -175,18 +194,26 @@
   <si>
     <t>(FEMALES)</t>
   </si>
+  <si>
+    <t>Labour  Force
+Participation  Rate  ( % )</t>
+  </si>
+  <si>
+    <t>Median  Age  of  Labour  Force
+( Years )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0;[Red]#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="7"/>
       <name val="Helv"/>
@@ -264,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -310,6 +337,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
@@ -318,7 +367,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -397,6 +446,30 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,30 +482,58 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="180"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_T10 (3)" xfId="4"/>
-    <cellStyle name="Normal_T2" xfId="2"/>
-    <cellStyle name="Normal_T2 (2)" xfId="3"/>
-    <cellStyle name="Normal_T3 (2)" xfId="1"/>
+    <cellStyle name="Normal_T10 (3)" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_T2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_T2 (2)" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal_T3 (2)" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -729,15 +830,1220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0E0983-B738-4A5D-B37E-9096BB8DC188}">
+  <sheetPr syncVertical="1" syncRef="A1" transitionEvaluation="1"/>
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.4"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="25" customFormat="1" ht="51">
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="22">
+        <v>1985.7</v>
+      </c>
+      <c r="C2" s="14">
+        <v>31.8</v>
+      </c>
+      <c r="D2" s="14">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="E2" s="9">
+        <v>220.7</v>
+      </c>
+      <c r="F2" s="9">
+        <v>248.3</v>
+      </c>
+      <c r="G2" s="9">
+        <v>268.89999999999998</v>
+      </c>
+      <c r="H2" s="14">
+        <v>263.2</v>
+      </c>
+      <c r="I2" s="9">
+        <v>262</v>
+      </c>
+      <c r="J2" s="9">
+        <v>233.2</v>
+      </c>
+      <c r="K2" s="14">
+        <v>159.5</v>
+      </c>
+      <c r="L2" s="14">
+        <v>92.1</v>
+      </c>
+      <c r="M2" s="9">
+        <v>35.9</v>
+      </c>
+      <c r="N2" s="9">
+        <v>24</v>
+      </c>
+      <c r="O2" s="47">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="P2" s="47">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="22">
+        <v>2047.3</v>
+      </c>
+      <c r="C3" s="14">
+        <v>41.2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>157.6</v>
+      </c>
+      <c r="E3" s="9">
+        <v>223.2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>254.7</v>
+      </c>
+      <c r="G3" s="9">
+        <v>275</v>
+      </c>
+      <c r="H3" s="14">
+        <v>254.4</v>
+      </c>
+      <c r="I3" s="9">
+        <v>266.89999999999998</v>
+      </c>
+      <c r="J3" s="9">
+        <v>235.7</v>
+      </c>
+      <c r="K3" s="14">
+        <v>178.5</v>
+      </c>
+      <c r="L3" s="14">
+        <v>98.7</v>
+      </c>
+      <c r="M3" s="9">
+        <v>36</v>
+      </c>
+      <c r="N3" s="9">
+        <v>25.6</v>
+      </c>
+      <c r="O3" s="47">
+        <v>66.2</v>
+      </c>
+      <c r="P3" s="47">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A4" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="22">
+        <v>2080.1</v>
+      </c>
+      <c r="C4" s="14">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D4" s="14">
+        <v>162.1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>214.6</v>
+      </c>
+      <c r="F4" s="9">
+        <v>249.4</v>
+      </c>
+      <c r="G4" s="9">
+        <v>268.2</v>
+      </c>
+      <c r="H4" s="14">
+        <v>256.89999999999998</v>
+      </c>
+      <c r="I4" s="9">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="J4" s="9">
+        <v>246.9</v>
+      </c>
+      <c r="K4" s="14">
+        <v>187.8</v>
+      </c>
+      <c r="L4" s="14">
+        <v>114.5</v>
+      </c>
+      <c r="M4" s="9">
+        <v>45.1</v>
+      </c>
+      <c r="N4" s="9">
+        <v>31.2</v>
+      </c>
+      <c r="O4" s="47">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="P4" s="47">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A5" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="22">
+        <v>2119.6</v>
+      </c>
+      <c r="C5" s="14">
+        <v>33.9</v>
+      </c>
+      <c r="D5" s="14">
+        <v>171.3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>207.3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>245</v>
+      </c>
+      <c r="G5" s="9">
+        <v>266.3</v>
+      </c>
+      <c r="H5" s="14">
+        <v>265.60000000000002</v>
+      </c>
+      <c r="I5" s="9">
+        <v>269.5</v>
+      </c>
+      <c r="J5" s="9">
+        <v>249.2</v>
+      </c>
+      <c r="K5" s="14">
+        <v>197</v>
+      </c>
+      <c r="L5" s="14">
+        <v>127.7</v>
+      </c>
+      <c r="M5" s="9">
+        <v>53.1</v>
+      </c>
+      <c r="N5" s="9">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="O5" s="47">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="P5" s="47">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A6" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2138.8000000000002</v>
+      </c>
+      <c r="C6" s="14">
+        <v>31.3</v>
+      </c>
+      <c r="D6" s="14">
+        <v>157.1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>209.7</v>
+      </c>
+      <c r="F6" s="9">
+        <v>248.6</v>
+      </c>
+      <c r="G6" s="9">
+        <v>262.3</v>
+      </c>
+      <c r="H6" s="14">
+        <v>266.3</v>
+      </c>
+      <c r="I6" s="9">
+        <v>266.3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>255.2</v>
+      </c>
+      <c r="K6" s="14">
+        <v>205.3</v>
+      </c>
+      <c r="L6" s="14">
+        <v>136.9</v>
+      </c>
+      <c r="M6" s="9">
+        <v>61.4</v>
+      </c>
+      <c r="N6" s="9">
+        <v>38.5</v>
+      </c>
+      <c r="O6" s="47">
+        <v>66.7</v>
+      </c>
+      <c r="P6" s="47">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="22">
+        <v>2185.1999999999998</v>
+      </c>
+      <c r="C7" s="14">
+        <v>31</v>
+      </c>
+      <c r="D7" s="14">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>217.6</v>
+      </c>
+      <c r="F7" s="9">
+        <v>250.1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>256.2</v>
+      </c>
+      <c r="H7" s="14">
+        <v>265.89999999999998</v>
+      </c>
+      <c r="I7" s="9">
+        <v>253</v>
+      </c>
+      <c r="J7" s="9">
+        <v>260.5</v>
+      </c>
+      <c r="K7" s="14">
+        <v>220.3</v>
+      </c>
+      <c r="L7" s="14">
+        <v>150.69999999999999</v>
+      </c>
+      <c r="M7" s="9">
+        <v>74.2</v>
+      </c>
+      <c r="N7" s="9">
+        <v>44.5</v>
+      </c>
+      <c r="O7" s="47">
+        <v>67</v>
+      </c>
+      <c r="P7" s="47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A8" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="22">
+        <v>2232.3000000000002</v>
+      </c>
+      <c r="C8" s="14">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="D8" s="14">
+        <v>166.2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>219.4</v>
+      </c>
+      <c r="F8" s="9">
+        <v>243.7</v>
+      </c>
+      <c r="G8" s="9">
+        <v>266.8</v>
+      </c>
+      <c r="H8" s="14">
+        <v>276</v>
+      </c>
+      <c r="I8" s="9">
+        <v>258.60000000000002</v>
+      </c>
+      <c r="J8" s="9">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="K8" s="14">
+        <v>223.7</v>
+      </c>
+      <c r="L8" s="14">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="M8" s="9">
+        <v>78.3</v>
+      </c>
+      <c r="N8" s="9">
+        <v>42</v>
+      </c>
+      <c r="O8" s="47">
+        <v>68.3</v>
+      </c>
+      <c r="P8" s="47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="22">
+        <v>2257.6</v>
+      </c>
+      <c r="C9" s="14">
+        <v>37.9</v>
+      </c>
+      <c r="D9" s="14">
+        <v>162.5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>239.3</v>
+      </c>
+      <c r="F9" s="9">
+        <v>244.7</v>
+      </c>
+      <c r="G9" s="9">
+        <v>259.7</v>
+      </c>
+      <c r="H9" s="14">
+        <v>268.39999999999998</v>
+      </c>
+      <c r="I9" s="9">
+        <v>260.10000000000002</v>
+      </c>
+      <c r="J9" s="9">
+        <v>262.3</v>
+      </c>
+      <c r="K9" s="14">
+        <v>226.9</v>
+      </c>
+      <c r="L9" s="14">
+        <v>164.1</v>
+      </c>
+      <c r="M9" s="9">
+        <v>87.9</v>
+      </c>
+      <c r="N9" s="9">
+        <v>43.9</v>
+      </c>
+      <c r="O9" s="47">
+        <v>68</v>
+      </c>
+      <c r="P9" s="47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A10" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="22">
+        <v>2269.6999999999998</v>
+      </c>
+      <c r="C10" s="14">
+        <v>35</v>
+      </c>
+      <c r="D10" s="14">
+        <v>153.19999999999999</v>
+      </c>
+      <c r="E10" s="9">
+        <v>229.3</v>
+      </c>
+      <c r="F10" s="9">
+        <v>242.4</v>
+      </c>
+      <c r="G10" s="9">
+        <v>275</v>
+      </c>
+      <c r="H10" s="14">
+        <v>281.10000000000002</v>
+      </c>
+      <c r="I10" s="9">
+        <v>272.39999999999998</v>
+      </c>
+      <c r="J10" s="9">
+        <v>254.8</v>
+      </c>
+      <c r="K10" s="14">
+        <v>213.6</v>
+      </c>
+      <c r="L10" s="14">
+        <v>166.5</v>
+      </c>
+      <c r="M10" s="9">
+        <v>92.1</v>
+      </c>
+      <c r="N10" s="9">
+        <v>54.4</v>
+      </c>
+      <c r="O10" s="47">
+        <v>67.7</v>
+      </c>
+      <c r="P10" s="47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A11" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="22">
+        <v>2292.6999999999998</v>
+      </c>
+      <c r="C11" s="14">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D11" s="14">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="E11" s="9">
+        <v>236.7</v>
+      </c>
+      <c r="F11" s="9">
+        <v>241.2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>270.7</v>
+      </c>
+      <c r="H11" s="14">
+        <v>278.39999999999998</v>
+      </c>
+      <c r="I11" s="9">
+        <v>270.89999999999998</v>
+      </c>
+      <c r="J11" s="9">
+        <v>259.8</v>
+      </c>
+      <c r="K11" s="14">
+        <v>224.5</v>
+      </c>
+      <c r="L11" s="14">
+        <v>170.9</v>
+      </c>
+      <c r="M11" s="9">
+        <v>93.7</v>
+      </c>
+      <c r="N11" s="9">
+        <v>56.9</v>
+      </c>
+      <c r="O11" s="47">
+        <v>67.7</v>
+      </c>
+      <c r="P11" s="47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A12" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="22">
+        <v>2328.5</v>
+      </c>
+      <c r="C12" s="14">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="D12" s="14">
+        <v>148.9</v>
+      </c>
+      <c r="E12" s="9">
+        <v>239</v>
+      </c>
+      <c r="F12" s="9">
+        <v>253.7</v>
+      </c>
+      <c r="G12" s="9">
+        <v>266.7</v>
+      </c>
+      <c r="H12" s="14">
+        <v>270.10000000000002</v>
+      </c>
+      <c r="I12" s="9">
+        <v>284.10000000000002</v>
+      </c>
+      <c r="J12" s="9">
+        <v>256.8</v>
+      </c>
+      <c r="K12" s="14">
+        <v>237.1</v>
+      </c>
+      <c r="L12" s="14">
+        <v>170.2</v>
+      </c>
+      <c r="M12" s="9">
+        <v>103.7</v>
+      </c>
+      <c r="N12" s="9">
+        <v>62.1</v>
+      </c>
+      <c r="O12" s="48">
+        <v>68</v>
+      </c>
+      <c r="P12" s="48">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1"/>
+    <row r="14" spans="1:16" s="7" customFormat="1" ht="24" customHeight="1"/>
+  </sheetData>
+  <conditionalFormatting sqref="B1:N12">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O12">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions gridLinesSet="0"/>
+  <pageMargins left="0.39370078740157483" right="0.74803149606299213" top="0.9055118110236221" bottom="0.9055118110236221" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450F73A-345C-4E59-8637-B8D7F45A5172}">
+  <sheetPr syncVertical="1" syncRef="A1" transitionEvaluation="1"/>
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.4"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="11" style="2" customWidth="1"/>
+    <col min="10" max="12" width="11" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="25" customFormat="1" ht="31.8" customHeight="1">
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="22">
+        <v>1985.7</v>
+      </c>
+      <c r="C2" s="22">
+        <v>2047.3</v>
+      </c>
+      <c r="D2" s="22">
+        <v>2080.1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>2119.6</v>
+      </c>
+      <c r="F2" s="22">
+        <v>2138.8000000000002</v>
+      </c>
+      <c r="G2" s="22">
+        <v>2185.1999999999998</v>
+      </c>
+      <c r="H2" s="22">
+        <v>2232.3000000000002</v>
+      </c>
+      <c r="I2" s="22">
+        <v>2257.6</v>
+      </c>
+      <c r="J2" s="22">
+        <v>2269.6999999999998</v>
+      </c>
+      <c r="K2" s="22">
+        <v>2292.6999999999998</v>
+      </c>
+      <c r="L2" s="22">
+        <v>2328.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="14">
+        <v>31.8</v>
+      </c>
+      <c r="C3" s="14">
+        <v>41.2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E3" s="14">
+        <v>33.9</v>
+      </c>
+      <c r="F3" s="14">
+        <v>31.3</v>
+      </c>
+      <c r="G3" s="14">
+        <v>31</v>
+      </c>
+      <c r="H3" s="14">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="I3" s="14">
+        <v>37.9</v>
+      </c>
+      <c r="J3" s="14">
+        <v>35</v>
+      </c>
+      <c r="K3" s="14">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="L3" s="14">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="C4" s="14">
+        <v>157.6</v>
+      </c>
+      <c r="D4" s="14">
+        <v>162.1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>171.3</v>
+      </c>
+      <c r="F4" s="14">
+        <v>157.1</v>
+      </c>
+      <c r="G4" s="14">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="H4" s="14">
+        <v>166.2</v>
+      </c>
+      <c r="I4" s="14">
+        <v>162.5</v>
+      </c>
+      <c r="J4" s="14">
+        <v>153.19999999999999</v>
+      </c>
+      <c r="K4" s="14">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="L4" s="14">
+        <v>148.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>220.7</v>
+      </c>
+      <c r="C5" s="9">
+        <v>223.2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>214.6</v>
+      </c>
+      <c r="E5" s="9">
+        <v>207.3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>209.7</v>
+      </c>
+      <c r="G5" s="9">
+        <v>217.6</v>
+      </c>
+      <c r="H5" s="9">
+        <v>219.4</v>
+      </c>
+      <c r="I5" s="9">
+        <v>239.3</v>
+      </c>
+      <c r="J5" s="9">
+        <v>229.3</v>
+      </c>
+      <c r="K5" s="9">
+        <v>236.7</v>
+      </c>
+      <c r="L5" s="9">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>248.3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>254.7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>249.4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>245</v>
+      </c>
+      <c r="F6" s="9">
+        <v>248.6</v>
+      </c>
+      <c r="G6" s="9">
+        <v>250.1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>243.7</v>
+      </c>
+      <c r="I6" s="9">
+        <v>244.7</v>
+      </c>
+      <c r="J6" s="9">
+        <v>242.4</v>
+      </c>
+      <c r="K6" s="9">
+        <v>241.2</v>
+      </c>
+      <c r="L6" s="9">
+        <v>253.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9">
+        <v>268.89999999999998</v>
+      </c>
+      <c r="C7" s="9">
+        <v>275</v>
+      </c>
+      <c r="D7" s="9">
+        <v>268.2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>266.3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>262.3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>256.2</v>
+      </c>
+      <c r="H7" s="9">
+        <v>266.8</v>
+      </c>
+      <c r="I7" s="9">
+        <v>259.7</v>
+      </c>
+      <c r="J7" s="9">
+        <v>275</v>
+      </c>
+      <c r="K7" s="9">
+        <v>270.7</v>
+      </c>
+      <c r="L7" s="9">
+        <v>266.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="14">
+        <v>263.2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>254.4</v>
+      </c>
+      <c r="D8" s="14">
+        <v>256.89999999999998</v>
+      </c>
+      <c r="E8" s="14">
+        <v>265.60000000000002</v>
+      </c>
+      <c r="F8" s="14">
+        <v>266.3</v>
+      </c>
+      <c r="G8" s="14">
+        <v>265.89999999999998</v>
+      </c>
+      <c r="H8" s="14">
+        <v>276</v>
+      </c>
+      <c r="I8" s="14">
+        <v>268.39999999999998</v>
+      </c>
+      <c r="J8" s="14">
+        <v>281.10000000000002</v>
+      </c>
+      <c r="K8" s="14">
+        <v>278.39999999999998</v>
+      </c>
+      <c r="L8" s="14">
+        <v>270.10000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <v>262</v>
+      </c>
+      <c r="C9" s="9">
+        <v>266.89999999999998</v>
+      </c>
+      <c r="D9" s="9">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="E9" s="9">
+        <v>269.5</v>
+      </c>
+      <c r="F9" s="9">
+        <v>266.3</v>
+      </c>
+      <c r="G9" s="9">
+        <v>253</v>
+      </c>
+      <c r="H9" s="9">
+        <v>258.60000000000002</v>
+      </c>
+      <c r="I9" s="9">
+        <v>260.10000000000002</v>
+      </c>
+      <c r="J9" s="9">
+        <v>272.39999999999998</v>
+      </c>
+      <c r="K9" s="9">
+        <v>270.89999999999998</v>
+      </c>
+      <c r="L9" s="9">
+        <v>284.10000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>233.2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>235.7</v>
+      </c>
+      <c r="D10" s="9">
+        <v>246.9</v>
+      </c>
+      <c r="E10" s="9">
+        <v>249.2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>255.2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>260.5</v>
+      </c>
+      <c r="H10" s="9">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="I10" s="9">
+        <v>262.3</v>
+      </c>
+      <c r="J10" s="9">
+        <v>254.8</v>
+      </c>
+      <c r="K10" s="9">
+        <v>259.8</v>
+      </c>
+      <c r="L10" s="9">
+        <v>256.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14">
+        <v>159.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>178.5</v>
+      </c>
+      <c r="D11" s="14">
+        <v>187.8</v>
+      </c>
+      <c r="E11" s="14">
+        <v>197</v>
+      </c>
+      <c r="F11" s="14">
+        <v>205.3</v>
+      </c>
+      <c r="G11" s="14">
+        <v>220.3</v>
+      </c>
+      <c r="H11" s="14">
+        <v>223.7</v>
+      </c>
+      <c r="I11" s="14">
+        <v>226.9</v>
+      </c>
+      <c r="J11" s="14">
+        <v>213.6</v>
+      </c>
+      <c r="K11" s="14">
+        <v>224.5</v>
+      </c>
+      <c r="L11" s="14">
+        <v>237.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="14">
+        <v>92.1</v>
+      </c>
+      <c r="C12" s="14">
+        <v>98.7</v>
+      </c>
+      <c r="D12" s="14">
+        <v>114.5</v>
+      </c>
+      <c r="E12" s="14">
+        <v>127.7</v>
+      </c>
+      <c r="F12" s="14">
+        <v>136.9</v>
+      </c>
+      <c r="G12" s="14">
+        <v>150.69999999999999</v>
+      </c>
+      <c r="H12" s="14">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="I12" s="14">
+        <v>164.1</v>
+      </c>
+      <c r="J12" s="14">
+        <v>166.5</v>
+      </c>
+      <c r="K12" s="14">
+        <v>170.9</v>
+      </c>
+      <c r="L12" s="14">
+        <v>170.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9">
+        <v>35.9</v>
+      </c>
+      <c r="C13" s="9">
+        <v>36</v>
+      </c>
+      <c r="D13" s="9">
+        <v>45.1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>53.1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>61.4</v>
+      </c>
+      <c r="G13" s="9">
+        <v>74.2</v>
+      </c>
+      <c r="H13" s="9">
+        <v>78.3</v>
+      </c>
+      <c r="I13" s="9">
+        <v>87.9</v>
+      </c>
+      <c r="J13" s="9">
+        <v>92.1</v>
+      </c>
+      <c r="K13" s="9">
+        <v>93.7</v>
+      </c>
+      <c r="L13" s="9">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9">
+        <v>25.6</v>
+      </c>
+      <c r="D14" s="9">
+        <v>31.2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="F14" s="9">
+        <v>38.5</v>
+      </c>
+      <c r="G14" s="9">
+        <v>44.5</v>
+      </c>
+      <c r="H14" s="9">
+        <v>42</v>
+      </c>
+      <c r="I14" s="9">
+        <v>43.9</v>
+      </c>
+      <c r="J14" s="9">
+        <v>54.4</v>
+      </c>
+      <c r="K14" s="9">
+        <v>56.9</v>
+      </c>
+      <c r="L14" s="9">
+        <v>62.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:L14">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions gridLinesSet="0"/>
+  <pageMargins left="0.39370078740157483" right="0.74803149606299213" top="0.9055118110236221" bottom="0.9055118110236221" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr syncVertical="1" syncRef="A1" transitionEvaluation="1"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Z1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.4"/>
   <cols>
     <col min="1" max="1" width="11" style="3" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
@@ -768,7 +2074,7 @@
     <col min="27" max="16384" width="9.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="21"/>
       <c r="B1" s="37" t="s">
         <v>30</v>
@@ -798,7 +2104,7 @@
       <c r="Y1" s="37"/>
       <c r="Z1" s="37"/>
     </row>
-    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="21"/>
       <c r="B2" s="37" t="s">
         <v>29</v>
@@ -828,7 +2134,7 @@
       <c r="Y2" s="37"/>
       <c r="Z2" s="37"/>
     </row>
-    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="38" t="s">
         <v>28</v>
@@ -858,7 +2164,7 @@
       <c r="Y3" s="38"/>
       <c r="Z3" s="38"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" s="21"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -888,59 +2194,59 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1">
       <c r="A5" s="21"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31" t="s">
+      <c r="J5" s="39"/>
+      <c r="K5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="39"/>
+      <c r="M5" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31" t="s">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31" t="s">
+      <c r="R5" s="39"/>
+      <c r="S5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31" t="s">
+      <c r="T5" s="39"/>
+      <c r="U5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31" t="s">
+      <c r="V5" s="39"/>
+      <c r="W5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31" t="s">
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="32"/>
-    </row>
-    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z5" s="40"/>
+    </row>
+    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="18"/>
       <c r="C6" s="24" t="s">
@@ -992,7 +2298,7 @@
       </c>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="21"/>
       <c r="B7" s="19"/>
       <c r="C7" s="12"/>
@@ -1044,7 +2350,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A8" s="20"/>
       <c r="B8" s="19"/>
       <c r="C8" s="12"/>
@@ -1096,7 +2402,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="20"/>
       <c r="B9" s="19"/>
       <c r="C9" s="12"/>
@@ -1148,7 +2454,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A10" s="20"/>
       <c r="B10" s="19"/>
       <c r="C10" s="12"/>
@@ -1200,7 +2506,7 @@
       </c>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A11" s="20"/>
       <c r="B11" s="19"/>
       <c r="C11" s="12"/>
@@ -1252,7 +2558,7 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A12" s="20"/>
       <c r="B12" s="19"/>
       <c r="C12" s="12"/>
@@ -1304,7 +2610,7 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A13" s="36" t="s">
         <v>7</v>
       </c>
@@ -1358,7 +2664,7 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
       <c r="A14" s="36"/>
       <c r="B14" s="18"/>
       <c r="C14" s="12"/>
@@ -1410,7 +2716,7 @@
       </c>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A15" s="36"/>
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
@@ -1462,7 +2768,7 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A16" s="36"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
@@ -1514,7 +2820,7 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A17" s="36"/>
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
@@ -1566,7 +2872,7 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A18" s="36"/>
       <c r="B18" s="13"/>
       <c r="C18" s="12"/>
@@ -1618,7 +2924,7 @@
       </c>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="19.95" customHeight="1">
       <c r="A19" s="36"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1668,7 +2974,7 @@
     <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:Z18">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1682,8 +2988,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr syncVertical="1" syncRef="A1" transitionEvaluation="1"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -1691,7 +2997,7 @@
       <selection activeCell="B1" sqref="B1:Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.4"/>
   <cols>
     <col min="1" max="1" width="11" style="3" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
@@ -1722,8 +3028,8 @@
     <col min="27" max="16384" width="9.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="37" t="s">
@@ -1754,8 +3060,8 @@
       <c r="Y1" s="37"/>
       <c r="Z1" s="37"/>
     </row>
-    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
+    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
+      <c r="A2" s="44"/>
       <c r="B2" s="37" t="s">
         <v>29</v>
       </c>
@@ -1784,8 +3090,8 @@
       <c r="Y2" s="37"/>
       <c r="Z2" s="37"/>
     </row>
-    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
+    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
+      <c r="A3" s="44"/>
       <c r="B3" s="38" t="s">
         <v>31</v>
       </c>
@@ -1814,8 +3120,8 @@
       <c r="Y3" s="38"/>
       <c r="Z3" s="38"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+    <row r="4" spans="1:26" ht="15" customHeight="1">
+      <c r="A4" s="44"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1844,60 +3150,60 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31" t="s">
+      <c r="J5" s="39"/>
+      <c r="K5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="39"/>
+      <c r="M5" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31" t="s">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31" t="s">
+      <c r="R5" s="39"/>
+      <c r="S5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31" t="s">
+      <c r="T5" s="39"/>
+      <c r="U5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31" t="s">
+      <c r="V5" s="39"/>
+      <c r="W5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31" t="s">
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="32"/>
-    </row>
-    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+      <c r="Z5" s="40"/>
+    </row>
+    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A6" s="44"/>
       <c r="B6" s="18"/>
       <c r="C6" s="24" t="s">
         <v>14</v>
@@ -1948,8 +3254,8 @@
       </c>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A7" s="44"/>
       <c r="B7" s="19"/>
       <c r="C7" s="12"/>
       <c r="D7" s="11" t="s">
@@ -2000,8 +3306,8 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A8" s="44"/>
       <c r="B8" s="19"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11" t="s">
@@ -2052,7 +3358,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="20"/>
       <c r="B9" s="19"/>
       <c r="C9" s="12"/>
@@ -2104,7 +3410,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A10" s="20"/>
       <c r="B10" s="19"/>
       <c r="C10" s="12"/>
@@ -2156,7 +3462,7 @@
       </c>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A11" s="20"/>
       <c r="B11" s="19"/>
       <c r="C11" s="12"/>
@@ -2208,7 +3514,7 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A12" s="20"/>
       <c r="B12" s="19"/>
       <c r="C12" s="12"/>
@@ -2260,7 +3566,7 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A13" s="20"/>
       <c r="B13" s="13"/>
       <c r="C13" s="12"/>
@@ -2312,7 +3618,7 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
       <c r="A14" s="20"/>
       <c r="B14" s="18"/>
       <c r="C14" s="12"/>
@@ -2364,7 +3670,7 @@
       </c>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A15" s="20"/>
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
@@ -2416,7 +3722,7 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A16" s="20"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
@@ -2468,7 +3774,7 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A17" s="30"/>
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
@@ -2520,7 +3826,7 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A18" s="30"/>
       <c r="B18" s="13"/>
       <c r="C18" s="12"/>
@@ -2572,7 +3878,7 @@
       </c>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="19.95" customHeight="1">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -2621,7 +3927,7 @@
     <mergeCell ref="S5:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:Z18">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2635,8 +3941,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr syncVertical="1" syncRef="A1" transitionEvaluation="1"/>
   <dimension ref="A1:Z19"/>
   <sheetViews>
@@ -2644,7 +3950,7 @@
       <selection activeCell="B1" sqref="B1:Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="11.4"/>
   <cols>
     <col min="1" max="1" width="11" style="3" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="1" customWidth="1"/>
@@ -2675,7 +3981,7 @@
     <col min="27" max="16384" width="9.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="21"/>
       <c r="B1" s="37" t="s">
         <v>32</v>
@@ -2705,7 +4011,7 @@
       <c r="Y1" s="37"/>
       <c r="Z1" s="37"/>
     </row>
-    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="21"/>
       <c r="B2" s="37" t="s">
         <v>29</v>
@@ -2735,7 +4041,7 @@
       <c r="Y2" s="37"/>
       <c r="Z2" s="37"/>
     </row>
-    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="29" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="38" t="s">
         <v>35</v>
@@ -2765,7 +4071,7 @@
       <c r="Y3" s="38"/>
       <c r="Z3" s="38"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" s="21"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
@@ -2795,59 +4101,59 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="25" customFormat="1" ht="32.25" customHeight="1">
       <c r="A5" s="21"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31" t="s">
+      <c r="J5" s="39"/>
+      <c r="K5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="39"/>
+      <c r="M5" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31" t="s">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31" t="s">
+      <c r="R5" s="39"/>
+      <c r="S5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31" t="s">
+      <c r="T5" s="39"/>
+      <c r="U5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31" t="s">
+      <c r="V5" s="39"/>
+      <c r="W5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31" t="s">
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="32"/>
-    </row>
-    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z5" s="40"/>
+    </row>
+    <row r="6" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="18"/>
       <c r="C6" s="24" t="s">
@@ -2899,7 +4205,7 @@
       </c>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="21"/>
       <c r="B7" s="19"/>
       <c r="C7" s="12"/>
@@ -2951,7 +4257,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A8" s="20"/>
       <c r="B8" s="19"/>
       <c r="C8" s="12"/>
@@ -3003,7 +4309,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="20"/>
       <c r="B9" s="19"/>
       <c r="C9" s="12"/>
@@ -3055,7 +4361,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A10" s="20"/>
       <c r="B10" s="19"/>
       <c r="C10" s="12"/>
@@ -3107,7 +4413,7 @@
       </c>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A11" s="20"/>
       <c r="B11" s="19"/>
       <c r="C11" s="12"/>
@@ -3159,8 +4465,8 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+    <row r="12" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A12" s="45" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="19"/>
@@ -3213,8 +4519,8 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A13" s="45"/>
       <c r="B13" s="13"/>
       <c r="C13" s="12"/>
       <c r="D13" s="11" t="s">
@@ -3265,8 +4571,8 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+    <row r="14" spans="1:26" s="16" customFormat="1" ht="24" customHeight="1">
+      <c r="A14" s="45"/>
       <c r="B14" s="18"/>
       <c r="C14" s="12"/>
       <c r="D14" s="11" t="s">
@@ -3317,8 +4623,8 @@
       </c>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+    <row r="15" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A15" s="45"/>
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
       <c r="D15" s="11" t="s">
@@ -3369,8 +4675,8 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+    <row r="16" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A16" s="45"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
       <c r="D16" s="11" t="s">
@@ -3421,8 +4727,8 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+    <row r="17" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A17" s="45"/>
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
       <c r="D17" s="11" t="s">
@@ -3473,8 +4779,8 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+    <row r="18" spans="1:26" s="7" customFormat="1" ht="24" customHeight="1">
+      <c r="A18" s="45"/>
       <c r="B18" s="13"/>
       <c r="C18" s="12"/>
       <c r="D18" s="11" t="s">
@@ -3525,8 +4831,8 @@
       </c>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+    <row r="19" spans="1:26" ht="19.95" customHeight="1">
+      <c r="A19" s="45"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -3575,7 +4881,7 @@
     <mergeCell ref="W5:X5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:Z18">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3590,65 +4896,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">4XQ4D5TRQRHF-1623496119-513</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">
-      <Url>https://stats.mom.gov.sg/_layouts/DocIdRedir.aspx?ID=4XQ4D5TRQRHF-1623496119-513</Url>
-      <Description>4XQ4D5TRQRHF-1623496119-513</Description>
-    </_dlc_DocIdUrl>
-    <_dlc_DocIdPersistId xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">false</_dlc_DocIdPersistId>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010061D1B60B48AE2C4381B419F34A85A18B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b8f4c4eb7c0a6ed6c0ddc723c58efda0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5775c44-5034-46ee-b1b0-8650967f43ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cab69d6e76fd2b3e146ab9f966a16f43" ns2:_="">
     <xsd:import namespace="e5775c44-5034-46ee-b1b0-8650967f43ea"/>
@@ -3793,6 +5040,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">4XQ4D5TRQRHF-1623496119-513</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">
+      <Url>https://stats.mom.gov.sg/_layouts/DocIdRedir.aspx?ID=4XQ4D5TRQRHF-1623496119-513</Url>
+      <Description>4XQ4D5TRQRHF-1623496119-513</Description>
+    </_dlc_DocIdUrl>
+    <_dlc_DocIdPersistId xmlns="e5775c44-5034-46ee-b1b0-8650967f43ea">false</_dlc_DocIdPersistId>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3803,17 +5109,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E1E5D72-9892-47A0-9CF5-D028A56D85BD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAEED2B2-05D4-485F-B584-85E02A07031E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e5775c44-5034-46ee-b1b0-8650967f43ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5659AF47-3969-414A-99B6-9C74532F53F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5659AF47-3969-414A-99B6-9C74532F53F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAEED2B2-05D4-485F-B584-85E02A07031E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E1E5D72-9892-47A0-9CF5-D028A56D85BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e5775c44-5034-46ee-b1b0-8650967f43ea"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DA4E5D-EB12-48EB-A7F5-D814CBC28E36}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DA4E5D-EB12-48EB-A7F5-D814CBC28E36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>